<commit_message>
Pattern Programs Exercise - 14th June
</commit_message>
<xml_diff>
--- a/PatternPrograms.xlsx
+++ b/PatternPrograms.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\OneDrive\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50325DF-CC4F-4A7E-971E-7A573552067B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC98603E-439E-4ED7-9922-BEFEEF4416A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{6F33D858-FDF9-43A6-AF06-937AFD7684D8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="6" xr2:uid="{6F33D858-FDF9-43A6-AF06-937AFD7684D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Type1" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,8 @@
     <sheet name="TYpe4" sheetId="4" r:id="rId4"/>
     <sheet name="Type5" sheetId="5" r:id="rId5"/>
     <sheet name="Type6" sheetId="6" r:id="rId6"/>
+    <sheet name="Exercise" sheetId="7" r:id="rId7"/>
+    <sheet name="Programs" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="470" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="144">
   <si>
     <t>*</t>
   </si>
@@ -445,13 +447,34 @@
   </si>
   <si>
     <t>2*3 -1</t>
+  </si>
+  <si>
+    <t>5432*</t>
+  </si>
+  <si>
+    <t>543*1</t>
+  </si>
+  <si>
+    <t>54*21</t>
+  </si>
+  <si>
+    <t>5*321</t>
+  </si>
+  <si>
+    <t>*4321</t>
+  </si>
+  <si>
+    <t>Find Even  &amp; odd Numbers from Naturals Numbers 1-100</t>
+  </si>
+  <si>
+    <t>Find  prime numbers from Naturals Numbers 1-100</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -487,6 +510,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="16">
@@ -762,7 +792,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -888,67 +918,73 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2226,10 +2262,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="I2" s="47" t="s">
+      <c r="I2" s="52" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="47"/>
+      <c r="J2" s="52"/>
     </row>
     <row r="3" spans="2:15" x14ac:dyDescent="0.3">
       <c r="I3" s="23" t="s">
@@ -3627,12 +3663,12 @@
       <c r="C1" t="s">
         <v>94</v>
       </c>
-      <c r="J1" s="48" t="s">
+      <c r="J1" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="53"/>
     </row>
     <row r="2" spans="2:14" x14ac:dyDescent="0.3">
       <c r="J2" t="s">
@@ -3819,12 +3855,12 @@
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="J11" s="48" t="s">
+      <c r="J11" s="53" t="s">
         <v>49</v>
       </c>
-      <c r="K11" s="48"/>
-      <c r="L11" s="48"/>
-      <c r="M11" s="48"/>
+      <c r="K11" s="53"/>
+      <c r="L11" s="53"/>
+      <c r="M11" s="53"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.3">
       <c r="J12" t="s">
@@ -4011,12 +4047,12 @@
       </c>
     </row>
     <row r="22" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="J22" s="48" t="s">
+      <c r="J22" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="K22" s="48"/>
-      <c r="L22" s="48"/>
-      <c r="M22" s="48"/>
+      <c r="K22" s="53"/>
+      <c r="L22" s="53"/>
+      <c r="M22" s="53"/>
     </row>
     <row r="23" spans="2:16" x14ac:dyDescent="0.3">
       <c r="J23" t="s">
@@ -4450,19 +4486,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="72" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="47" t="s">
+      <c r="B1" s="52" t="s">
         <v>93</v>
       </c>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
       <c r="F1" s="42" t="s">
         <v>95</v>
       </c>
-      <c r="H1" s="56" t="s">
+      <c r="H1" s="55" t="s">
         <v>97</v>
       </c>
-      <c r="I1" s="56"/>
+      <c r="I1" s="55"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="H2" s="15" t="s">
@@ -4488,10 +4524,10 @@
       <c r="I3" s="40" t="s">
         <v>91</v>
       </c>
-      <c r="L3" s="51" t="s">
+      <c r="L3" s="57" t="s">
         <v>98</v>
       </c>
-      <c r="M3" s="52"/>
+      <c r="M3" s="58"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B4" s="45">
@@ -4503,7 +4539,7 @@
       <c r="D4" s="45"/>
       <c r="E4" s="45"/>
       <c r="F4" s="15"/>
-      <c r="G4" s="49" t="s">
+      <c r="G4" s="56" t="s">
         <v>98</v>
       </c>
       <c r="H4" s="41">
@@ -4512,16 +4548,16 @@
       <c r="I4" s="41">
         <v>1</v>
       </c>
-      <c r="J4" s="49" t="s">
+      <c r="J4" s="56" t="s">
         <v>92</v>
       </c>
       <c r="L4" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="M4" s="53" t="s">
+      <c r="M4" s="59" t="s">
         <v>101</v>
       </c>
-      <c r="N4" s="49" t="s">
+      <c r="N4" s="56" t="s">
         <v>104</v>
       </c>
     </row>
@@ -4537,19 +4573,19 @@
       </c>
       <c r="E5" s="45"/>
       <c r="F5" s="15"/>
-      <c r="G5" s="49"/>
+      <c r="G5" s="56"/>
       <c r="H5" s="41">
         <v>2</v>
       </c>
       <c r="I5" s="41">
         <v>2</v>
       </c>
-      <c r="J5" s="49"/>
+      <c r="J5" s="56"/>
       <c r="L5" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="M5" s="55"/>
-      <c r="N5" s="49"/>
+      <c r="M5" s="61"/>
+      <c r="N5" s="56"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="B6" s="45">
@@ -4564,19 +4600,19 @@
       <c r="E6" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="G6" s="49"/>
+      <c r="G6" s="56"/>
       <c r="H6" s="41">
         <v>3</v>
       </c>
       <c r="I6" s="41">
         <v>3</v>
       </c>
-      <c r="J6" s="49"/>
+      <c r="J6" s="56"/>
       <c r="L6" s="44" t="s">
         <v>103</v>
       </c>
-      <c r="M6" s="54"/>
-      <c r="N6" s="49"/>
+      <c r="M6" s="60"/>
+      <c r="N6" s="56"/>
     </row>
     <row r="7" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B7" s="11">
@@ -4590,7 +4626,7 @@
       </c>
       <c r="E7" s="14"/>
       <c r="F7" s="15"/>
-      <c r="G7" s="49" t="s">
+      <c r="G7" s="56" t="s">
         <v>99</v>
       </c>
       <c r="H7" s="14">
@@ -4599,14 +4635,14 @@
       <c r="I7" s="14">
         <v>2</v>
       </c>
-      <c r="J7" s="49" t="s">
+      <c r="J7" s="56" t="s">
         <v>96</v>
       </c>
       <c r="L7" s="43" t="s">
         <v>107</v>
       </c>
       <c r="M7" s="43"/>
-      <c r="N7" s="53" t="s">
+      <c r="N7" s="59" t="s">
         <v>105</v>
       </c>
     </row>
@@ -4620,26 +4656,26 @@
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
       <c r="F8" s="15"/>
-      <c r="G8" s="49"/>
+      <c r="G8" s="56"/>
       <c r="H8" s="14">
         <v>5</v>
       </c>
       <c r="I8" s="14">
         <v>1</v>
       </c>
-      <c r="J8" s="49"/>
+      <c r="J8" s="56"/>
       <c r="L8" s="43" t="s">
         <v>106</v>
       </c>
       <c r="M8" s="43"/>
-      <c r="N8" s="54"/>
+      <c r="N8" s="60"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="I12" s="43"/>
-      <c r="J12" s="50" t="s">
+      <c r="J12" s="62" t="s">
         <v>97</v>
       </c>
-      <c r="K12" s="50"/>
+      <c r="K12" s="62"/>
       <c r="L12" s="43"/>
       <c r="M12" s="43"/>
       <c r="N12" s="43"/>
@@ -4692,10 +4728,10 @@
       <c r="M14" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="N14" s="49" t="s">
+      <c r="N14" s="56" t="s">
         <v>98</v>
       </c>
-      <c r="O14" s="49"/>
+      <c r="O14" s="56"/>
       <c r="P14" s="43"/>
       <c r="Q14" s="43"/>
       <c r="R14" s="40" t="s">
@@ -4709,7 +4745,7 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A15" s="57" t="s">
+      <c r="A15" s="54" t="s">
         <v>121</v>
       </c>
       <c r="B15" s="11">
@@ -4722,7 +4758,7 @@
       <c r="E15" s="14"/>
       <c r="F15" s="43"/>
       <c r="G15" s="43"/>
-      <c r="I15" s="49" t="s">
+      <c r="I15" s="56" t="s">
         <v>98</v>
       </c>
       <c r="J15" s="41">
@@ -4731,7 +4767,7 @@
       <c r="K15" s="41">
         <v>1</v>
       </c>
-      <c r="L15" s="49" t="s">
+      <c r="L15" s="56" t="s">
         <v>108</v>
       </c>
       <c r="M15" s="43" t="s">
@@ -4740,8 +4776,8 @@
       <c r="N15" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="O15" s="49"/>
-      <c r="P15" s="49" t="s">
+      <c r="O15" s="56"/>
+      <c r="P15" s="56" t="s">
         <v>104</v>
       </c>
       <c r="Q15" s="43"/>
@@ -4756,7 +4792,7 @@
       </c>
     </row>
     <row r="16" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="57"/>
+      <c r="A16" s="54"/>
       <c r="B16" s="11">
         <v>2</v>
       </c>
@@ -4771,22 +4807,22 @@
       </c>
       <c r="F16" s="43"/>
       <c r="G16" s="43"/>
-      <c r="I16" s="49"/>
+      <c r="I16" s="56"/>
       <c r="J16" s="41">
         <v>2</v>
       </c>
       <c r="K16" s="41">
         <v>3</v>
       </c>
-      <c r="L16" s="49"/>
+      <c r="L16" s="56"/>
       <c r="M16" s="43" t="s">
         <v>111</v>
       </c>
       <c r="N16" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="O16" s="49"/>
-      <c r="P16" s="49"/>
+      <c r="O16" s="56"/>
+      <c r="P16" s="56"/>
       <c r="Q16" s="43"/>
       <c r="R16" s="41">
         <v>2</v>
@@ -4799,7 +4835,7 @@
       </c>
     </row>
     <row r="17" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="57"/>
+      <c r="A17" s="54"/>
       <c r="B17" s="11">
         <v>3</v>
       </c>
@@ -4818,22 +4854,22 @@
       <c r="G17" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="I17" s="49"/>
+      <c r="I17" s="56"/>
       <c r="J17" s="41">
         <v>3</v>
       </c>
       <c r="K17" s="41">
         <v>5</v>
       </c>
-      <c r="L17" s="49"/>
+      <c r="L17" s="56"/>
       <c r="M17" s="43" t="s">
         <v>112</v>
       </c>
       <c r="N17" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="O17" s="49"/>
-      <c r="P17" s="49"/>
+      <c r="O17" s="56"/>
+      <c r="P17" s="56"/>
       <c r="Q17" s="43"/>
       <c r="R17" s="41">
         <v>3</v>
@@ -4846,7 +4882,7 @@
       </c>
     </row>
     <row r="18" spans="1:20" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A18" s="57" t="s">
+      <c r="A18" s="54" t="s">
         <v>122</v>
       </c>
       <c r="B18" s="11">
@@ -4863,7 +4899,7 @@
       </c>
       <c r="F18" s="43"/>
       <c r="G18" s="43"/>
-      <c r="I18" s="49" t="s">
+      <c r="I18" s="56" t="s">
         <v>99</v>
       </c>
       <c r="J18" s="14">
@@ -4872,7 +4908,7 @@
       <c r="K18" s="14">
         <v>3</v>
       </c>
-      <c r="L18" s="49" t="s">
+      <c r="L18" s="56" t="s">
         <v>96</v>
       </c>
       <c r="M18" s="46" t="s">
@@ -4882,13 +4918,13 @@
         <v>107</v>
       </c>
       <c r="O18" s="43"/>
-      <c r="P18" s="49" t="s">
+      <c r="P18" s="56" t="s">
         <v>105</v>
       </c>
       <c r="Q18" s="43"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A19" s="57"/>
+      <c r="A19" s="54"/>
       <c r="B19" s="11">
         <v>5</v>
       </c>
@@ -4899,14 +4935,14 @@
       <c r="E19" s="14"/>
       <c r="F19" s="43"/>
       <c r="G19" s="43"/>
-      <c r="I19" s="49"/>
+      <c r="I19" s="56"/>
       <c r="J19" s="14">
         <v>5</v>
       </c>
       <c r="K19" s="14">
         <v>1</v>
       </c>
-      <c r="L19" s="49"/>
+      <c r="L19" s="56"/>
       <c r="M19" s="46" t="s">
         <v>114</v>
       </c>
@@ -4914,7 +4950,7 @@
         <v>106</v>
       </c>
       <c r="O19" s="43"/>
-      <c r="P19" s="49"/>
+      <c r="P19" s="56"/>
       <c r="Q19" s="43"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.3">
@@ -5026,18 +5062,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="H1:I1"/>
-    <mergeCell ref="J7:J8"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="N4:N6"/>
-    <mergeCell ref="N7:N8"/>
-    <mergeCell ref="M4:M6"/>
-    <mergeCell ref="J4:J6"/>
     <mergeCell ref="L18:L19"/>
     <mergeCell ref="P18:P19"/>
     <mergeCell ref="J12:K12"/>
@@ -5047,6 +5071,18 @@
     <mergeCell ref="O15:O17"/>
     <mergeCell ref="P15:P17"/>
     <mergeCell ref="I18:I19"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="N4:N6"/>
+    <mergeCell ref="N7:N8"/>
+    <mergeCell ref="M4:M6"/>
+    <mergeCell ref="J4:J6"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J7:J8"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="G7:G8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5057,7 +5093,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EE29222-880E-42B5-8227-55803C9192C2}">
   <dimension ref="B2:T61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+    <sheetView topLeftCell="A49" workbookViewId="0">
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
@@ -5068,26 +5104,26 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:20" x14ac:dyDescent="0.3">
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="56" t="s">
         <v>128</v>
       </c>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="J2" s="61" t="s">
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="J2" s="63" t="s">
         <v>125</v>
       </c>
-      <c r="K2" s="62"/>
-      <c r="L2" s="63"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="65"/>
     </row>
     <row r="3" spans="2:20" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="60"/>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="J3" s="61" t="s">
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="J3" s="63" t="s">
         <v>132</v>
       </c>
-      <c r="K3" s="62"/>
-      <c r="L3" s="63"/>
+      <c r="K3" s="64"/>
+      <c r="L3" s="65"/>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.3">
       <c r="B5" s="16" t="s">
@@ -5108,31 +5144,31 @@
       <c r="G5" s="11">
         <v>5</v>
       </c>
-      <c r="J5" s="59" t="s">
+      <c r="J5" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="59" t="s">
+      <c r="K5" s="48" t="s">
         <v>134</v>
       </c>
-      <c r="L5" s="59" t="s">
+      <c r="L5" s="48" t="s">
         <v>124</v>
       </c>
-      <c r="N5" s="59" t="s">
+      <c r="N5" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="O5" s="59" t="s">
+      <c r="O5" s="48" t="s">
         <v>123</v>
       </c>
-      <c r="P5" s="67" t="s">
+      <c r="P5" s="51" t="s">
         <v>133</v>
       </c>
-      <c r="R5" s="59" t="s">
+      <c r="R5" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="S5" s="59" t="s">
+      <c r="S5" s="48" t="s">
         <v>124</v>
       </c>
-      <c r="T5" s="67" t="s">
+      <c r="T5" s="51" t="s">
         <v>89</v>
       </c>
     </row>
@@ -5140,38 +5176,38 @@
       <c r="B6" s="11">
         <v>1</v>
       </c>
-      <c r="C6" s="58"/>
-      <c r="D6" s="58"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
       <c r="E6" s="45" t="s">
         <v>0</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
-      <c r="I6" s="64" t="s">
+      <c r="I6" s="66" t="s">
         <v>126</v>
       </c>
-      <c r="J6" s="65">
-        <v>1</v>
-      </c>
-      <c r="K6" s="65">
-        <v>2</v>
-      </c>
-      <c r="L6" s="65">
-        <v>1</v>
-      </c>
-      <c r="N6" s="65">
-        <v>1</v>
-      </c>
-      <c r="O6" s="65">
+      <c r="J6" s="49">
+        <v>1</v>
+      </c>
+      <c r="K6" s="49">
+        <v>2</v>
+      </c>
+      <c r="L6" s="49">
+        <v>1</v>
+      </c>
+      <c r="N6" s="49">
+        <v>1</v>
+      </c>
+      <c r="O6" s="49">
         <v>2</v>
       </c>
       <c r="P6" s="34" t="s">
         <v>129</v>
       </c>
-      <c r="R6" s="65">
-        <v>1</v>
-      </c>
-      <c r="S6" s="65">
+      <c r="R6" s="49">
+        <v>1</v>
+      </c>
+      <c r="S6" s="49">
         <v>1</v>
       </c>
       <c r="T6" t="s">
@@ -5182,7 +5218,7 @@
       <c r="B7" s="11">
         <v>2</v>
       </c>
-      <c r="C7" s="58"/>
+      <c r="C7" s="47"/>
       <c r="D7" s="45" t="s">
         <v>0</v>
       </c>
@@ -5193,29 +5229,29 @@
         <v>0</v>
       </c>
       <c r="G7" s="5"/>
-      <c r="I7" s="64"/>
-      <c r="J7" s="65">
-        <v>2</v>
-      </c>
-      <c r="K7" s="65">
-        <v>1</v>
-      </c>
-      <c r="L7" s="65">
-        <v>3</v>
-      </c>
-      <c r="N7" s="65">
-        <v>2</v>
-      </c>
-      <c r="O7" s="65">
+      <c r="I7" s="66"/>
+      <c r="J7" s="49">
+        <v>2</v>
+      </c>
+      <c r="K7" s="49">
+        <v>1</v>
+      </c>
+      <c r="L7" s="49">
+        <v>3</v>
+      </c>
+      <c r="N7" s="49">
+        <v>2</v>
+      </c>
+      <c r="O7" s="49">
         <v>1</v>
       </c>
       <c r="P7" s="34" t="s">
         <v>130</v>
       </c>
-      <c r="R7" s="65">
-        <v>2</v>
-      </c>
-      <c r="S7" s="65">
+      <c r="R7" s="49">
+        <v>2</v>
+      </c>
+      <c r="S7" s="49">
         <v>3</v>
       </c>
       <c r="T7" t="s">
@@ -5241,29 +5277,29 @@
       <c r="G8" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="I8" s="64"/>
-      <c r="J8" s="65">
-        <v>3</v>
-      </c>
-      <c r="K8" s="65">
-        <v>0</v>
-      </c>
-      <c r="L8" s="65">
-        <v>5</v>
-      </c>
-      <c r="N8" s="65">
-        <v>3</v>
-      </c>
-      <c r="O8" s="65">
+      <c r="I8" s="66"/>
+      <c r="J8" s="49">
+        <v>3</v>
+      </c>
+      <c r="K8" s="49">
+        <v>0</v>
+      </c>
+      <c r="L8" s="49">
+        <v>5</v>
+      </c>
+      <c r="N8" s="49">
+        <v>3</v>
+      </c>
+      <c r="O8" s="49">
         <v>0</v>
       </c>
       <c r="P8" s="34" t="s">
         <v>131</v>
       </c>
-      <c r="R8" s="65">
-        <v>3</v>
-      </c>
-      <c r="S8" s="65">
+      <c r="R8" s="49">
+        <v>3</v>
+      </c>
+      <c r="S8" s="49">
         <v>5</v>
       </c>
       <c r="T8" t="s">
@@ -5274,7 +5310,7 @@
       <c r="B9" s="11">
         <v>4</v>
       </c>
-      <c r="C9" s="58"/>
+      <c r="C9" s="47"/>
       <c r="D9" s="45" t="s">
         <v>0</v>
       </c>
@@ -5285,16 +5321,16 @@
         <v>0</v>
       </c>
       <c r="G9" s="5"/>
-      <c r="I9" s="64" t="s">
+      <c r="I9" s="66" t="s">
         <v>127</v>
       </c>
-      <c r="J9" s="66">
-        <v>4</v>
-      </c>
-      <c r="K9" s="66">
-        <v>1</v>
-      </c>
-      <c r="L9" s="66">
+      <c r="J9" s="50">
+        <v>4</v>
+      </c>
+      <c r="K9" s="50">
+        <v>1</v>
+      </c>
+      <c r="L9" s="50">
         <v>3</v>
       </c>
     </row>
@@ -5302,21 +5338,21 @@
       <c r="B10" s="11">
         <v>5</v>
       </c>
-      <c r="C10" s="58"/>
-      <c r="D10" s="58"/>
+      <c r="C10" s="47"/>
+      <c r="D10" s="47"/>
       <c r="E10" s="45" t="s">
         <v>0</v>
       </c>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
-      <c r="I10" s="64"/>
-      <c r="J10" s="66">
-        <v>5</v>
-      </c>
-      <c r="K10" s="66">
-        <v>2</v>
-      </c>
-      <c r="L10" s="66">
+      <c r="I10" s="66"/>
+      <c r="J10" s="50">
+        <v>5</v>
+      </c>
+      <c r="K10" s="50">
+        <v>2</v>
+      </c>
+      <c r="L10" s="50">
         <v>1</v>
       </c>
     </row>
@@ -5344,8 +5380,8 @@
       <c r="B16" s="11">
         <v>1</v>
       </c>
-      <c r="C16" s="58"/>
-      <c r="D16" s="58"/>
+      <c r="C16" s="47"/>
+      <c r="D16" s="47"/>
       <c r="E16" s="45" t="s">
         <v>52</v>
       </c>
@@ -5356,7 +5392,7 @@
       <c r="B17" s="11">
         <v>2</v>
       </c>
-      <c r="C17" s="58"/>
+      <c r="C17" s="47"/>
       <c r="D17" s="45" t="s">
         <v>53</v>
       </c>
@@ -5392,7 +5428,7 @@
       <c r="B19" s="11">
         <v>4</v>
       </c>
-      <c r="C19" s="58"/>
+      <c r="C19" s="47"/>
       <c r="D19" s="45" t="s">
         <v>55</v>
       </c>
@@ -5408,8 +5444,8 @@
       <c r="B20" s="11">
         <v>5</v>
       </c>
-      <c r="C20" s="58"/>
-      <c r="D20" s="58"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="47"/>
       <c r="E20" s="45" t="s">
         <v>56</v>
       </c>
@@ -5440,8 +5476,8 @@
       <c r="B26" s="11">
         <v>1</v>
       </c>
-      <c r="C26" s="58"/>
-      <c r="D26" s="58"/>
+      <c r="C26" s="47"/>
+      <c r="D26" s="47"/>
       <c r="E26" s="45">
         <v>1</v>
       </c>
@@ -5452,7 +5488,7 @@
       <c r="B27" s="11">
         <v>2</v>
       </c>
-      <c r="C27" s="58"/>
+      <c r="C27" s="47"/>
       <c r="D27" s="45">
         <v>2</v>
       </c>
@@ -5488,7 +5524,7 @@
       <c r="B29" s="11">
         <v>4</v>
       </c>
-      <c r="C29" s="58"/>
+      <c r="C29" s="47"/>
       <c r="D29" s="45">
         <v>4</v>
       </c>
@@ -5504,8 +5540,8 @@
       <c r="B30" s="11">
         <v>5</v>
       </c>
-      <c r="C30" s="58"/>
-      <c r="D30" s="58"/>
+      <c r="C30" s="47"/>
+      <c r="D30" s="47"/>
       <c r="E30" s="45">
         <v>5</v>
       </c>
@@ -5536,8 +5572,8 @@
       <c r="B36" s="11">
         <v>1</v>
       </c>
-      <c r="C36" s="58"/>
-      <c r="D36" s="58"/>
+      <c r="C36" s="47"/>
+      <c r="D36" s="47"/>
       <c r="E36" s="45" t="s">
         <v>52</v>
       </c>
@@ -5548,7 +5584,7 @@
       <c r="B37" s="11">
         <v>2</v>
       </c>
-      <c r="C37" s="58"/>
+      <c r="C37" s="47"/>
       <c r="D37" s="45" t="s">
         <v>53</v>
       </c>
@@ -5584,7 +5620,7 @@
       <c r="B39" s="11">
         <v>4</v>
       </c>
-      <c r="C39" s="58"/>
+      <c r="C39" s="47"/>
       <c r="D39" s="45" t="s">
         <v>61</v>
       </c>
@@ -5600,8 +5636,8 @@
       <c r="B40" s="11">
         <v>5</v>
       </c>
-      <c r="C40" s="58"/>
-      <c r="D40" s="58"/>
+      <c r="C40" s="47"/>
+      <c r="D40" s="47"/>
       <c r="E40" s="45" t="s">
         <v>64</v>
       </c>
@@ -5632,8 +5668,8 @@
       <c r="B47" s="11">
         <v>1</v>
       </c>
-      <c r="C47" s="58"/>
-      <c r="D47" s="58"/>
+      <c r="C47" s="47"/>
+      <c r="D47" s="47"/>
       <c r="E47" s="45">
         <v>1</v>
       </c>
@@ -5644,7 +5680,7 @@
       <c r="B48" s="11">
         <v>2</v>
       </c>
-      <c r="C48" s="58"/>
+      <c r="C48" s="47"/>
       <c r="D48" s="45">
         <v>2</v>
       </c>
@@ -5680,7 +5716,7 @@
       <c r="B50" s="11">
         <v>4</v>
       </c>
-      <c r="C50" s="58"/>
+      <c r="C50" s="47"/>
       <c r="D50" s="45">
         <v>10</v>
       </c>
@@ -5696,8 +5732,8 @@
       <c r="B51" s="11">
         <v>5</v>
       </c>
-      <c r="C51" s="58"/>
-      <c r="D51" s="58"/>
+      <c r="C51" s="47"/>
+      <c r="D51" s="47"/>
       <c r="E51" s="45">
         <v>13</v>
       </c>
@@ -5728,8 +5764,8 @@
       <c r="B57" s="11">
         <v>1</v>
       </c>
-      <c r="C57" s="58"/>
-      <c r="D57" s="58"/>
+      <c r="C57" s="47"/>
+      <c r="D57" s="47"/>
       <c r="E57" s="45" t="s">
         <v>0</v>
       </c>
@@ -5740,7 +5776,7 @@
       <c r="B58" s="11">
         <v>2</v>
       </c>
-      <c r="C58" s="58"/>
+      <c r="C58" s="47"/>
       <c r="D58" s="45" t="s">
         <v>0</v>
       </c>
@@ -5770,7 +5806,7 @@
       <c r="B60" s="11">
         <v>4</v>
       </c>
-      <c r="C60" s="58"/>
+      <c r="C60" s="47"/>
       <c r="D60" s="45" t="s">
         <v>0</v>
       </c>
@@ -5784,8 +5820,8 @@
       <c r="B61" s="11">
         <v>5</v>
       </c>
-      <c r="C61" s="58"/>
-      <c r="D61" s="58"/>
+      <c r="C61" s="47"/>
+      <c r="D61" s="47"/>
       <c r="E61" s="45" t="s">
         <v>0</v>
       </c>
@@ -5804,4 +5840,103 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31C0D7B6-5DB0-47FD-A648-70A402AAEB59}">
+  <dimension ref="B4:F17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="22" customWidth="1"/>
+    <col min="6" max="6" width="47.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B4" s="68" t="s">
+        <v>137</v>
+      </c>
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B5" s="68" t="s">
+        <v>138</v>
+      </c>
+      <c r="E5" s="5">
+        <v>2</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B6" s="68" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B7" s="68" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B8" s="68" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B13" s="69">
+        <v>55555</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B14" s="69">
+        <v>45555</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B15" s="69">
+        <v>34555</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B16" s="69">
+        <v>23455</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" ht="16.8" x14ac:dyDescent="0.3">
+      <c r="B17" s="69">
+        <v>12345</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ACC15D7-3889-4440-8DB7-C2B7B4B2FAAF}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="97.33203125" customWidth="1"/>
+  </cols>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>